<commit_message>
Ajustes a factor de flex y maq de estado
</commit_message>
<xml_diff>
--- a/Sistema-Embebido/Maquina de estados - Inputs y States.xlsx
+++ b/Sistema-Embebido/Maquina de estados - Inputs y States.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VSIFRSCA\Desktop\Franco\Facultad\Sistemas Operativos Avanzados\TP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VSIFRSCA\Documents\eclipse-workspace\X1\Sistema-Embebido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{2FECC3B5-4312-4D8D-AFD4-1B9F07DB4366}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782DB72-8456-44E6-B832-AF4190606E8C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7665ADB3-6E5E-47B9-9E94-1D2C781CEA02}"/>
+    <workbookView xWindow="12330" yWindow="1785" windowWidth="15375" windowHeight="7875" xr2:uid="{7665ADB3-6E5E-47B9-9E94-1D2C781CEA02}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>StarPZ</t>
   </si>
@@ -112,6 +112,33 @@
   </si>
   <si>
     <t>InDefault</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>PLAY</t>
+  </si>
+  <si>
+    <t>PAUSE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>PLUS_10S</t>
+  </si>
+  <si>
+    <t>LESS_10S</t>
+  </si>
+  <si>
+    <t>PLUS_20S</t>
+  </si>
+  <si>
+    <t>no imprime</t>
   </si>
 </sst>
 </file>
@@ -161,15 +188,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B0B242-1382-4425-8274-15C37E6076F4}">
-  <dimension ref="B2:H30"/>
+  <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,21 +527,25 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -520,36 +554,40 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="E4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
@@ -558,24 +596,25 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
@@ -584,21 +623,25 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
@@ -607,18 +650,24 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
@@ -627,9 +676,12 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
@@ -638,18 +690,24 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="E13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
@@ -658,9 +716,12 @@
       <c r="D15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="E15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
@@ -669,9 +730,12 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
@@ -680,9 +744,12 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="s">
@@ -691,9 +758,12 @@
       <c r="D18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
@@ -702,9 +772,12 @@
       <c r="D19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
@@ -713,105 +786,79 @@
       <c r="D20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B20:B30"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B20:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed de comunicacion arduino-android
</commit_message>
<xml_diff>
--- a/Sistema-Embebido/Maquina de estados - Inputs y States.xlsx
+++ b/Sistema-Embebido/Maquina de estados - Inputs y States.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VSIFRSCA\Documents\eclipse-workspace\X1\Sistema-Embebido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782DB72-8456-44E6-B832-AF4190606E8C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DB8BC7-5F92-4CE8-AE8E-A3D544FB6BBF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12330" yWindow="1785" windowWidth="15375" windowHeight="7875" xr2:uid="{7665ADB3-6E5E-47B9-9E94-1D2C781CEA02}"/>
+    <workbookView xWindow="9360" yWindow="705" windowWidth="15375" windowHeight="7875" xr2:uid="{7665ADB3-6E5E-47B9-9E94-1D2C781CEA02}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>StarPZ</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>PLUS_20S</t>
-  </si>
-  <si>
-    <t>no imprime</t>
   </si>
 </sst>
 </file>
@@ -519,7 +516,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,9 +567,7 @@
       <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
@@ -853,12 +848,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B20:B25"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B20:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>